<commit_message>
Update Student - Prepopulating the HTML Form
</commit_message>
<xml_diff>
--- a/me_docs/12.Update Student.xlsx
+++ b/me_docs/12.Update Student.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B866087D-64EB-460A-8D0E-EDBDF7265A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EBDD18-5AF2-4E2D-953F-37D2A904AA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
     <sheet name="Creating the Update Link" sheetId="2" r:id="rId2"/>
+    <sheet name="Prepopulating the HTML Form" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Creating the Update Link list-students.jsp</t>
   </si>
@@ -35,6 +36,129 @@
   </si>
   <si>
     <t>Access URL to test</t>
+  </si>
+  <si>
+    <t>Create EditStudentControllerServlet</t>
+  </si>
+  <si>
+    <t>Init</t>
+  </si>
+  <si>
+    <t>doGet method</t>
+  </si>
+  <si>
+    <t>getStudent method in StudentDbUtil Class</t>
+  </si>
+  <si>
+    <t>public Student getStudent(String theStudentId) throws Exception {</t>
+  </si>
+  <si>
+    <t>Student theStudent = null;</t>
+  </si>
+  <si>
+    <t>Connection myConn = null;</t>
+  </si>
+  <si>
+    <t>PreparedStatement myStmt = null;</t>
+  </si>
+  <si>
+    <t>ResultSet myRs = null;</t>
+  </si>
+  <si>
+    <t>int studentId;</t>
+  </si>
+  <si>
+    <t>try {</t>
+  </si>
+  <si>
+    <t>// convert student id to int</t>
+  </si>
+  <si>
+    <t>studentId = Integer.parseInt(theStudentId);</t>
+  </si>
+  <si>
+    <t>// get connection to database</t>
+  </si>
+  <si>
+    <t>myConn = dataSource.getConnection();</t>
+  </si>
+  <si>
+    <t>// create sql to get selected student</t>
+  </si>
+  <si>
+    <t>String sql = "select * from student where id=?";</t>
+  </si>
+  <si>
+    <t>// create prepared statement</t>
+  </si>
+  <si>
+    <t>myStmt = myConn.prepareStatement(sql);</t>
+  </si>
+  <si>
+    <t>// set params</t>
+  </si>
+  <si>
+    <t>myStmt.setInt(1, studentId);</t>
+  </si>
+  <si>
+    <t>// execute statement</t>
+  </si>
+  <si>
+    <t>myRs = myStmt.executeQuery();</t>
+  </si>
+  <si>
+    <t>// retrieve data from result set row</t>
+  </si>
+  <si>
+    <t>if (myRs.next()) {</t>
+  </si>
+  <si>
+    <t>String firstName = myRs.getString("first_name");</t>
+  </si>
+  <si>
+    <t>String lastName = myRs.getString("last_name");</t>
+  </si>
+  <si>
+    <t>String email = myRs.getString("email");</t>
+  </si>
+  <si>
+    <t>// use the studentId during construction</t>
+  </si>
+  <si>
+    <t>theStudent = new Student(studentId, firstName, lastName, email);</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>else {</t>
+  </si>
+  <si>
+    <t>throw new Exception("Could not find student id: " + studentId);</t>
+  </si>
+  <si>
+    <t>return theStudent;</t>
+  </si>
+  <si>
+    <t>finally {</t>
+  </si>
+  <si>
+    <t>// clean up JDBC objects</t>
+  </si>
+  <si>
+    <t>close(myConn, myStmt, myRs);</t>
+  </si>
+  <si>
+    <t>All code</t>
+  </si>
+  <si>
+    <t>Add update-student-form.jsp</t>
+  </si>
+  <si>
+    <t>Restart Server</t>
+  </si>
+  <si>
+    <t>Edit page redirected</t>
   </si>
 </sst>
 </file>
@@ -264,6 +388,759 @@
         <a:xfrm>
           <a:off x="609600" y="12001500"/>
           <a:ext cx="9390476" cy="4352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161067</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB6FDC84-9F10-4E94-8BAD-535BA5CCB786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6866667" cy="5095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C035A3FE-F37C-4AFA-B08D-5444AD275E3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="4876190" cy="3628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C979417-1BEF-409E-9076-562516DB8954}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9525000"/>
+          <a:ext cx="4876190" cy="4638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>56571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{306A267C-D7D6-4B57-8CE1-4D8F014B051B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14287500"/>
+          <a:ext cx="4866667" cy="4628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>141409</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>123190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF130F7-E52A-4F91-A6B2-0641B10B502E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19240500"/>
+          <a:ext cx="11723809" cy="5076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>84267</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE4FD3A-CA10-48BD-8691-DDAAEC2AFF97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24574500"/>
+          <a:ext cx="11666667" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>112838</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>123048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA54D63F-3A74-4D16-8612-77CC6CC8EAD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="29908500"/>
+          <a:ext cx="11695238" cy="6219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>36647</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>85095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23705846-F90B-457B-8479-AA027F13F04C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="36576000"/>
+          <a:ext cx="11619047" cy="5038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>103238</xdr:colOff>
+      <xdr:row>331</xdr:row>
+      <xdr:rowOff>94619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A275399D-440E-4287-8BEF-DB00C8466E34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="42100500"/>
+          <a:ext cx="12295238" cy="5047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>436647</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>142238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96375048-72F7-4AB8-AECF-62A509A91CF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47434500"/>
+          <a:ext cx="12019047" cy="5095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>46171</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>66048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33719CC4-A0E2-4B26-BFB0-CBFB2B90159F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="41910000"/>
+          <a:ext cx="11628571" cy="5019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>560381</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>75571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924AAE96-607F-4709-B865-3FA9EB5DD7AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47244000"/>
+          <a:ext cx="12752381" cy="5028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>131886</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>123190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333E6091-9C34-43AD-A388-E1FAE8B6FD60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52578000"/>
+          <a:ext cx="11714286" cy="5076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>151238</xdr:colOff>
+      <xdr:row>443</xdr:row>
+      <xdr:rowOff>18286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75581095-5B6D-4BBD-B18E-1B1EB53F1A32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="78486000"/>
+          <a:ext cx="9295238" cy="6114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>446</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>37409</xdr:colOff>
+      <xdr:row>470</xdr:row>
+      <xdr:rowOff>142286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA0F9A30-72A7-4155-B2B5-4525A7C4391B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="84963000"/>
+          <a:ext cx="5523809" cy="4714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>473</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>284571</xdr:colOff>
+      <xdr:row>492</xdr:row>
+      <xdr:rowOff>56690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{053E1EA5-A03B-4CEB-A0CD-8015AEA66B8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="90106500"/>
+          <a:ext cx="9428571" cy="3676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>494</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>75581</xdr:colOff>
+      <xdr:row>515</xdr:row>
+      <xdr:rowOff>104262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C00A22-DE26-43A7-9FE8-A85E53395AD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="94107000"/>
+          <a:ext cx="4952381" cy="4104762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -555,7 +1432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E31CE5-BB8F-4191-9049-10FCE5ABF5FB}">
   <dimension ref="A2:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
@@ -580,4 +1457,250 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B86310E-794C-4845-9228-CD81A3C3EF2F}">
+  <dimension ref="A2:F494"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A458" workbookViewId="0">
+      <selection activeCell="M517" sqref="M517"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C363" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D364" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D366" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D367" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D368" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="369" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D369" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D371" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="372" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E372" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="373" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E373" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="375" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E375" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="376" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E376" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="378" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E378" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="379" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E379" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="381" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E381" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="382" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E382" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="384" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E384" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="385" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E385" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="387" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E387" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="388" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E388" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="390" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E390" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="391" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E391" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="392" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F392" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="393" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F393" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="394" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F394" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="396" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F396" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="397" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F397" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="398" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E398" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="399" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E399" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="400" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F400" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E401" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E403" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D404" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D405" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E406" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E407" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D408" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C409" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="494" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B494" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Student - Developing the Servlet
</commit_message>
<xml_diff>
--- a/me_docs/12.Update Student.xlsx
+++ b/me_docs/12.Update Student.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EBDD18-5AF2-4E2D-953F-37D2A904AA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15555445-B18A-4564-AB94-177A9368EA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
     <sheet name="Creating the Update Link" sheetId="2" r:id="rId2"/>
     <sheet name="Prepopulating the HTML Form" sheetId="3" r:id="rId3"/>
+    <sheet name="Developing the Servlet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Creating the Update Link list-students.jsp</t>
   </si>
@@ -159,6 +160,18 @@
   </si>
   <si>
     <t>Edit page redirected</t>
+  </si>
+  <si>
+    <t>doPost method</t>
+  </si>
+  <si>
+    <t>updateStudent created in StudentDbUtil class</t>
+  </si>
+  <si>
+    <t>Access Url to check do not anything after click save bottun on edit view, rediected to list view</t>
+  </si>
+  <si>
+    <t>List view</t>
   </si>
 </sst>
 </file>
@@ -1141,6 +1154,319 @@
         <a:xfrm>
           <a:off x="609600" y="94107000"/>
           <a:ext cx="4952381" cy="4104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>198552</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35C0E566-A18B-46CD-837B-9F7DBA4ADE02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="11780952" cy="5076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8076</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>104190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFCBF775-0329-4652-9101-214792508562}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="11590476" cy="4676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>255695</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>56429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA089A4-AC07-4EA6-B494-374F3A2BE868}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="10668000"/>
+          <a:ext cx="11838095" cy="5771429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>513143</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>18238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72216E58-9A13-4D54-8A15-C89CA87F772F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16954500"/>
+          <a:ext cx="9657143" cy="6495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323048</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>85190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BDE7697-846C-4B47-9BD3-35D60C894924}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23812500"/>
+          <a:ext cx="6419048" cy="4276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160762</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>180476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B19020-12AF-4856-92D0-7CA6E5860091}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="28384500"/>
+          <a:ext cx="9304762" cy="3990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>179809</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>161429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE59A764-0E7B-4155-9E69-0DAAB9181980}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32766000"/>
+          <a:ext cx="9323809" cy="3971429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1463,7 +1789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B86310E-794C-4845-9228-CD81A3C3EF2F}">
   <dimension ref="A2:F494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A458" workbookViewId="0">
+    <sheetView topLeftCell="A470" workbookViewId="0">
       <selection activeCell="M517" sqref="M517"/>
     </sheetView>
   </sheetViews>
@@ -1703,4 +2029,45 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C735159A-3B42-4638-A296-7E6BAEC0BF2F}">
+  <dimension ref="A2:B172"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Student - Creating the JDBC Code
</commit_message>
<xml_diff>
--- a/me_docs/12.Update Student.xlsx
+++ b/me_docs/12.Update Student.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15555445-B18A-4564-AB94-177A9368EA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A581ACD1-BDC6-4B74-B4CA-232E1745BE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
     <sheet name="Creating the Update Link" sheetId="2" r:id="rId2"/>
     <sheet name="Prepopulating the HTML Form" sheetId="3" r:id="rId3"/>
     <sheet name="Developing the Servlet" sheetId="4" r:id="rId4"/>
+    <sheet name="Creating the JDBC Code" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Creating the Update Link list-students.jsp</t>
   </si>
@@ -172,6 +173,15 @@
   </si>
   <si>
     <t>List view</t>
+  </si>
+  <si>
+    <t>updateStudent method in StudentDbUtil Class</t>
+  </si>
+  <si>
+    <t>doPost in EditStudentControllerServlet Class</t>
+  </si>
+  <si>
+    <t>Access Url to check</t>
   </si>
 </sst>
 </file>
@@ -1467,6 +1477,275 @@
         <a:xfrm>
           <a:off x="609600" y="32766000"/>
           <a:ext cx="9323809" cy="3971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>598857</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>75524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8202ADE-20C3-4203-8C6D-EEA3D82D210D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="9742857" cy="5409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>255695</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>104143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575A2181-9274-40B1-95BD-39BC3C8F8B70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6286500"/>
+          <a:ext cx="11838095" cy="5057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342248</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>47071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B107A631-7307-4399-B45E-2C7127E153DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11811000"/>
+          <a:ext cx="5219048" cy="4428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>151929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10212C7-E48F-45C4-8938-5F441DFFDAAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16764000"/>
+          <a:ext cx="9314286" cy="3771429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>113676</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>28071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB2D7BC7-2C69-49E5-BBBD-40087FE52545}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20764500"/>
+          <a:ext cx="4990476" cy="4028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>179809</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>75738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{923AB3AD-8B2D-4BD0-8128-14295653B324}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24955500"/>
+          <a:ext cx="9323809" cy="3695238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2035,7 +2314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C735159A-3B42-4638-A296-7E6BAEC0BF2F}">
   <dimension ref="A2:B172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+    <sheetView topLeftCell="A190" workbookViewId="0">
       <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
@@ -2070,4 +2349,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC88EE52-61C8-4382-9CBB-81C89E3690F3}">
+  <dimension ref="A2:A88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>